<commit_message>
experience and rejection template added
</commit_message>
<xml_diff>
--- a/Booktestold.xlsx
+++ b/Booktestold.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>ref</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>Chenle</t>
+  </si>
+  <si>
+    <t>January 1,2024</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>January 1,2022</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Software Engineer I</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -119,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -155,11 +173,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -167,6 +196,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,15 +392,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14"/>
+  <cols>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.9140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -387,8 +423,17 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.5">
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -405,8 +450,17 @@
         <v>4</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.5">
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -423,8 +477,17 @@
         <v>8</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.5">
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -443,8 +506,17 @@
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.5">
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -463,8 +535,17 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.5">
+      <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -483,17 +564,26 @@
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.5">
+      <c r="G6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="15.5">
+    <row r="9" spans="1:9" ht="15.5">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="15.5">
+    <row r="10" spans="1:9" ht="15.5">
       <c r="A10" s="2"/>
     </row>
   </sheetData>

</xml_diff>